<commit_message>
Split out string tests into it's own test suite
</commit_message>
<xml_diff>
--- a/reeevr/test/excelunit/reeevr-tests.xlsx
+++ b/reeevr/test/excelunit/reeevr-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mo14776\PycharmProjects\Excel-R-compiler\reeevr\test\excelunit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13D85F5-14B7-4F75-92EF-E7559D727B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B9AC90-2944-4DBB-BFFF-43FB1A6C7233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51741016-DE60-49DF-9826-25EB96E04CFB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>_xlfn.GAMMA.INV</t>
   </si>
@@ -59,69 +59,9 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>_xlfn.CONCAT</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>aBC</t>
-  </si>
-  <si>
-    <t>££$$</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>43ABCaBC££$$test21321</t>
-  </si>
-  <si>
-    <t>ABCaBC££$$test2132143ABCaBC££$$test21321</t>
-  </si>
-  <si>
-    <t>aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</t>
-  </si>
-  <si>
-    <t>££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</t>
-  </si>
-  <si>
-    <t>test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</t>
-  </si>
-  <si>
-    <t>2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</t>
-  </si>
-  <si>
-    <t>CONCATENATE</t>
-  </si>
-  <si>
-    <t>43ABC</t>
-  </si>
-  <si>
-    <t>ABCaBC</t>
-  </si>
-  <si>
-    <t>aBC££$$</t>
-  </si>
-  <si>
-    <t>££$$test</t>
-  </si>
-  <si>
-    <t>test21321</t>
-  </si>
-  <si>
-    <t>2132143ABC</t>
-  </si>
-  <si>
     <t>SUM</t>
   </si>
   <si>
-    <t>INDEX</t>
-  </si>
-  <si>
-    <t>CHOOSE</t>
-  </si>
-  <si>
     <t>COUNTA</t>
   </si>
   <si>
@@ -152,15 +92,6 @@
     <t>CEILING</t>
   </si>
   <si>
-    <t>LEFT</t>
-  </si>
-  <si>
-    <t>RIGHT</t>
-  </si>
-  <si>
-    <t>MID</t>
-  </si>
-  <si>
     <t>_xlfn.NORM.DIST</t>
   </si>
   <si>
@@ -204,51 +135,6 @@
   </si>
   <si>
     <t>MMULT</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Test and Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test </t>
-  </si>
-  <si>
-    <t>Test and T</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Test and</t>
-  </si>
-  <si>
-    <t>Te</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test</t>
-  </si>
-  <si>
-    <t>t and Test</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>and Test</t>
-  </si>
-  <si>
-    <t>st</t>
-  </si>
-  <si>
-    <t>st a</t>
-  </si>
-  <si>
-    <t>nd Test</t>
-  </si>
-  <si>
-    <t>and T</t>
   </si>
 </sst>
 </file>
@@ -629,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1FF9ED-8125-4F1D-B85A-69D7CAC66BA2}">
-  <dimension ref="B2:T54"/>
+  <dimension ref="B2:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +547,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -726,7 +612,7 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -791,7 +677,7 @@
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -856,7 +742,7 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -921,7 +807,7 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>0.1</v>
@@ -986,7 +872,7 @@
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0.1</v>
@@ -1051,7 +937,7 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -1116,7 +1002,7 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -1181,7 +1067,7 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1246,7 +1132,7 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -1311,7 +1197,7 @@
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -1397,27 +1283,27 @@
         <v>9</v>
       </c>
       <c r="I14">
-        <f>_xlfn.GAMMA.INV(0.25,C14,D14)</f>
+        <f t="shared" ref="I14:N14" si="10">_xlfn.GAMMA.INV(0.25,C14,D14)</f>
         <v>10.363796507163114</v>
       </c>
       <c r="J14">
-        <f>_xlfn.GAMMA.INV(0.25,D14,E14)</f>
+        <f t="shared" si="10"/>
         <v>21.096046915339478</v>
       </c>
       <c r="K14">
-        <f>_xlfn.GAMMA.INV(0.25,E14,F14)</f>
+        <f t="shared" si="10"/>
         <v>33.686003859773209</v>
       </c>
       <c r="L14">
-        <f>_xlfn.GAMMA.INV(0.25,F14,G14)</f>
+        <f t="shared" si="10"/>
         <v>19.701011262285849</v>
       </c>
       <c r="M14">
-        <f>_xlfn.GAMMA.INV(0.25,G14,H14)</f>
+        <f t="shared" si="10"/>
         <v>12.381772675515375</v>
       </c>
       <c r="N14">
-        <f>_xlfn.GAMMA.INV(0.25,H14,I14)</f>
+        <f t="shared" si="10"/>
         <v>70.863963183949636</v>
       </c>
       <c r="O14">
@@ -1462,27 +1348,27 @@
         <v>9</v>
       </c>
       <c r="I15">
-        <f>GAMMAINV(0.25,C15,D15)</f>
+        <f t="shared" ref="I15:N15" si="11">GAMMAINV(0.25,C15,D15)</f>
         <v>10.363796507163114</v>
       </c>
       <c r="J15">
-        <f>GAMMAINV(0.25,D15,E15)</f>
+        <f t="shared" si="11"/>
         <v>21.096046915339478</v>
       </c>
       <c r="K15">
-        <f>GAMMAINV(0.25,E15,F15)</f>
+        <f t="shared" si="11"/>
         <v>33.686003859773209</v>
       </c>
       <c r="L15">
-        <f>GAMMAINV(0.25,F15,G15)</f>
+        <f t="shared" si="11"/>
         <v>19.701011262285849</v>
       </c>
       <c r="M15">
-        <f>GAMMAINV(0.25,G15,H15)</f>
+        <f t="shared" si="11"/>
         <v>12.381772675515375</v>
       </c>
       <c r="N15">
-        <f>GAMMAINV(0.25,H15,I15)</f>
+        <f t="shared" si="11"/>
         <v>70.863963183949636</v>
       </c>
       <c r="O15">
@@ -1506,7 +1392,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1531,19 +1417,19 @@
         <v>0.23237459354875287</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:M16" si="10">_xlfn.LOGNORM.DIST(0.25,D16,E16,TRUE)</f>
+        <f t="shared" ref="J16:M16" si="12">_xlfn.LOGNORM.DIST(0.25,D16,E16,TRUE)</f>
         <v>6.9803129022922475E-2</v>
       </c>
       <c r="K16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.26153201360668754</v>
       </c>
       <c r="L16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.9994477654216036E-6</v>
       </c>
       <c r="M16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.33092295424797069</v>
       </c>
       <c r="N16">
@@ -1571,7 +1457,7 @@
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1592,27 +1478,27 @@
         <v>9</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17" si="11">_xlfn.LOGNORM.DIST(0.25,C17,D17,TRUE)</f>
+        <f t="shared" ref="I17" si="13">_xlfn.LOGNORM.DIST(0.25,C17,D17,TRUE)</f>
         <v>0.23237459354875287</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="J17" si="12">_xlfn.LOGNORM.DIST(0.25,D17,E17,TRUE)</f>
+        <f t="shared" ref="J17" si="14">_xlfn.LOGNORM.DIST(0.25,D17,E17,TRUE)</f>
         <v>6.9803129022922475E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17" si="13">_xlfn.LOGNORM.DIST(0.25,E17,F17,TRUE)</f>
+        <f t="shared" ref="K17" si="15">_xlfn.LOGNORM.DIST(0.25,E17,F17,TRUE)</f>
         <v>0.26153201360668754</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17" si="14">_xlfn.LOGNORM.DIST(0.25,F17,G17,TRUE)</f>
+        <f t="shared" ref="L17" si="16">_xlfn.LOGNORM.DIST(0.25,F17,G17,TRUE)</f>
         <v>3.9994477654216036E-6</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17" si="15">_xlfn.LOGNORM.DIST(0.25,G17,H17,TRUE)</f>
+        <f t="shared" ref="M17" si="17">_xlfn.LOGNORM.DIST(0.25,G17,H17,TRUE)</f>
         <v>0.33092295424797069</v>
       </c>
       <c r="N17">
-        <f t="shared" ref="N17" si="16">_xlfn.LOGNORM.DIST(0.25,H17,E17,TRUE)</f>
+        <f t="shared" ref="N17" si="18">_xlfn.LOGNORM.DIST(0.25,H17,E17,TRUE)</f>
         <v>1.8888836402617078E-2</v>
       </c>
       <c r="O17">
@@ -1636,7 +1522,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1661,19 +1547,19 @@
         <v>0.23237459354875287</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:M18" si="17">LOGNORMDIST(0.25,D18,E18)</f>
+        <f t="shared" ref="J18:M18" si="19">LOGNORMDIST(0.25,D18,E18)</f>
         <v>6.9803129022922475E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.26153201360668754</v>
       </c>
       <c r="L18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>3.9994477654216036E-6</v>
       </c>
       <c r="M18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.33092295424797069</v>
       </c>
       <c r="N18">
@@ -1701,7 +1587,7 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -1726,19 +1612,19 @@
         <v>4.6875000000000007E-2</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J19:M19" si="18">_xlfn.BINOM.DIST(D19,E19,0.25,FALSE)</f>
+        <f t="shared" ref="J19:M19" si="20">_xlfn.BINOM.DIST(D19,E19,0.25,FALSE)</f>
         <v>1.4648437500000005E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>5.8399200439453146E-2</v>
       </c>
       <c r="L19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.5405158996582038E-5</v>
       </c>
       <c r="M19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.1441297829151157E-5</v>
       </c>
       <c r="N19">
@@ -1766,7 +1652,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -1795,15 +1681,15 @@
         <v>0.9990234375</v>
       </c>
       <c r="K20">
-        <f t="shared" ref="K20" si="19">_xlfn.BINOM.DIST(E20,F20,0.25,TRUE)</f>
+        <f t="shared" ref="K20" si="21">_xlfn.BINOM.DIST(E20,F20,0.25,TRUE)</f>
         <v>0.98027229309082031</v>
       </c>
       <c r="L20">
-        <f t="shared" ref="L20" si="20">_xlfn.BINOM.DIST(F20,G20,0.25,TRUE)</f>
+        <f t="shared" ref="L20" si="22">_xlfn.BINOM.DIST(F20,G20,0.25,TRUE)</f>
         <v>0.99999779462814331</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20" si="21">_xlfn.BINOM.DIST(G20,H20,0.25,TRUE)</f>
+        <f t="shared" ref="M20" si="23">_xlfn.BINOM.DIST(G20,H20,0.25,TRUE)</f>
         <v>0.99999907705932856</v>
       </c>
       <c r="N20">
@@ -1831,7 +1717,7 @@
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -1856,19 +1742,19 @@
         <v>4.6875000000000007E-2</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:M21" si="22">BINOMDIST(D21,E21,0.25,FALSE)</f>
+        <f t="shared" ref="J21:M21" si="24">BINOMDIST(D21,E21,0.25,FALSE)</f>
         <v>1.4648437500000005E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>5.8399200439453146E-2</v>
       </c>
       <c r="L21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>3.5405158996582038E-5</v>
       </c>
       <c r="M21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.1441297829151157E-5</v>
       </c>
       <c r="N21">
@@ -1896,7 +1782,7 @@
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1921,19 +1807,19 @@
         <v>0.99609375</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22:M22" si="23">BINOMDIST(D22,E22,0.25,TRUE)</f>
+        <f t="shared" ref="J22:M22" si="25">BINOMDIST(D22,E22,0.25,TRUE)</f>
         <v>0.9990234375</v>
       </c>
       <c r="K22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.98027229309082031</v>
       </c>
       <c r="L22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.99999779462814331</v>
       </c>
       <c r="M22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.99999907705932856</v>
       </c>
       <c r="N22">
@@ -1961,7 +1847,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1986,19 +1872,19 @@
         <v>2.49169921875</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:M23" si="24">_xlfn.BETA.DIST(0.25,D23,E23,FALSE)</f>
+        <f t="shared" ref="J23:M23" si="26">_xlfn.BETA.DIST(0.25,D23,E23,FALSE)</f>
         <v>0.38932800292968761</v>
       </c>
       <c r="K23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>2.9359285533428183</v>
       </c>
       <c r="L23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>7.57019555594542E-4</v>
       </c>
       <c r="M23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>2.8200688274659864</v>
       </c>
       <c r="N23">
@@ -2026,7 +1912,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2051,11 +1937,11 @@
         <v>0.32145690917968756</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24:M24" si="25">_xlfn.BETA.DIST(0.25,D24,E24,TRUE)</f>
+        <f t="shared" ref="J24:M24" si="27">_xlfn.BETA.DIST(0.25,D24,E24,TRUE)</f>
         <v>1.9727706909179688E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.25846539810299879</v>
       </c>
       <c r="L24">
@@ -2063,7 +1949,7 @@
         <v>1.9827842592112129E-5</v>
       </c>
       <c r="M24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.6407501924257808</v>
       </c>
       <c r="N24">
@@ -2091,7 +1977,7 @@
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -2116,11 +2002,11 @@
         <v>3.6040220509731846E-3</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:K25" si="26">_xlfn.BETA.DIST(0.25,D25,E25,FALSE,0.2,5)</f>
+        <f t="shared" ref="J25:K25" si="28">_xlfn.BETA.DIST(0.25,D25,E25,FALSE,0.2,5)</f>
         <v>3.0873270036434237E-8</v>
       </c>
       <c r="K25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2.2344943362139383E-5</v>
       </c>
       <c r="L25">
@@ -2128,11 +2014,11 @@
         <v>1.8206766293043581E-7</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:N25" si="27">_xlfn.BETA.DIST(0.75,G25,H25,FALSE,0.2,5)</f>
+        <f t="shared" ref="M25:N25" si="29">_xlfn.BETA.DIST(0.75,G25,H25,FALSE,0.2,5)</f>
         <v>0.66151720230661659</v>
       </c>
       <c r="N25">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>2.5434860158670713E-11</v>
       </c>
       <c r="O25">
@@ -2156,7 +2042,7 @@
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -2181,23 +2067,23 @@
         <v>6.086408065798257E-5</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:N26" si="28">_xlfn.BETA.DIST(0.25,D26,E26,TRUE,0.2,5)</f>
+        <f t="shared" ref="J26:N26" si="30">_xlfn.BETA.DIST(0.25,D26,E26,TRUE,0.2,5)</f>
         <v>2.5883090562088557E-10</v>
       </c>
       <c r="K26">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>2.2702042015897622E-7</v>
       </c>
       <c r="L26">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.593935682745769E-19</v>
       </c>
       <c r="M26">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>7.8631448558295902E-4</v>
       </c>
       <c r="N26">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>9.8591655427125137E-24</v>
       </c>
       <c r="O26">
@@ -2221,7 +2107,7 @@
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -2246,23 +2132,23 @@
         <v>0.32145690917968756</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27:N27" si="29">BETADIST(0.25,D27,E27)</f>
+        <f t="shared" ref="J27:N27" si="31">BETADIST(0.25,D27,E27)</f>
         <v>1.9727706909179688E-2</v>
       </c>
       <c r="K27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.25846539810299879</v>
       </c>
       <c r="L27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>1.9827842592112129E-5</v>
       </c>
       <c r="M27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.6407501924257808</v>
       </c>
       <c r="N27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>3.6270505652248254E-7</v>
       </c>
       <c r="O27">
@@ -2286,7 +2172,7 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -2311,11 +2197,11 @@
         <v>6.086408065798257E-5</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28" si="30">_xlfn.BETA.DIST(0.25,D28,E28,FALSE,0.2,5)</f>
+        <f t="shared" ref="J28" si="32">_xlfn.BETA.DIST(0.25,D28,E28,FALSE,0.2,5)</f>
         <v>3.0873270036434237E-8</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28" si="31">_xlfn.BETA.DIST(0.25,E28,F28,FALSE,0.2,5)</f>
+        <f t="shared" ref="K28" si="33">_xlfn.BETA.DIST(0.25,E28,F28,FALSE,0.2,5)</f>
         <v>2.2344943362139383E-5</v>
       </c>
       <c r="L28">
@@ -2323,11 +2209,11 @@
         <v>1.8206766293043581E-7</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28" si="32">_xlfn.BETA.DIST(0.75,G28,H28,FALSE,0.2,5)</f>
+        <f t="shared" ref="M28" si="34">_xlfn.BETA.DIST(0.75,G28,H28,FALSE,0.2,5)</f>
         <v>0.66151720230661659</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28" si="33">_xlfn.BETA.DIST(0.75,H28,I28,FALSE,0.2,5)</f>
+        <f t="shared" ref="N28" si="35">_xlfn.BETA.DIST(0.75,H28,I28,FALSE,0.2,5)</f>
         <v>4.2561054174920979E-13</v>
       </c>
       <c r="O28">
@@ -2351,7 +2237,7 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -2376,11 +2262,11 @@
         <v>6.086408065798257E-5</v>
       </c>
       <c r="J29">
-        <f t="shared" ref="J29:N29" si="34">BETADIST(0.25,D29,E29,0.2,5)</f>
+        <f t="shared" ref="J29:N29" si="36">BETADIST(0.25,D29,E29,0.2,5)</f>
         <v>2.5883090562088557E-10</v>
       </c>
       <c r="K29">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>2.2702042015897622E-7</v>
       </c>
       <c r="L29">
@@ -2388,11 +2274,11 @@
         <v>4.593935682745769E-19</v>
       </c>
       <c r="M29">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>7.8631448558295902E-4</v>
       </c>
       <c r="N29">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>9.8591655427125137E-24</v>
       </c>
       <c r="O29">
@@ -2416,7 +2302,7 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -2441,19 +2327,19 @@
         <v>8.6799276445604517E-4</v>
       </c>
       <c r="J30">
-        <f t="shared" ref="J30:M30" si="35">_xlfn.WEIBULL.DIST(0.25,D30,E30,FALSE)</f>
+        <f t="shared" ref="J30:M30" si="37">_xlfn.WEIBULL.DIST(0.25,D30,E30,FALSE)</f>
         <v>3.7499999414062546E-7</v>
       </c>
       <c r="K30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1.9531249809265103E-7</v>
       </c>
       <c r="L30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>3.2813931992314361E-9</v>
       </c>
       <c r="M30">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1.0964330194305082E-3</v>
       </c>
       <c r="N30">
@@ -2481,7 +2367,7 @@
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -2506,19 +2392,19 @@
         <v>1.9512188925245291E-3</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31:M31" si="36">_xlfn.WEIBULL.DIST(0.75,D31,E31,TRUE)</f>
+        <f t="shared" ref="J31:M31" si="38">_xlfn.WEIBULL.DIST(0.75,D31,E31,TRUE)</f>
         <v>1.1390560127077369E-5</v>
       </c>
       <c r="K31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2.3730440593264908E-6</v>
       </c>
       <c r="L31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>4.8440629434220179E-6</v>
       </c>
       <c r="M31">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>1.768900592032779E-3</v>
       </c>
       <c r="N31">
@@ -2546,7 +2432,7 @@
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -2571,19 +2457,19 @@
         <v>8.6799276445604517E-4</v>
       </c>
       <c r="J32">
-        <f t="shared" ref="J32:M32" si="37">WEIBULL(0.25,D32,E32,FALSE)</f>
+        <f t="shared" ref="J32:M32" si="39">WEIBULL(0.25,D32,E32,FALSE)</f>
         <v>3.7499999414062546E-7</v>
       </c>
       <c r="K32">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1.9531249809265103E-7</v>
       </c>
       <c r="L32">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>3.2813931992314361E-9</v>
       </c>
       <c r="M32">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>1.0964330194305082E-3</v>
       </c>
       <c r="N32">
@@ -2611,7 +2497,7 @@
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -2636,19 +2522,19 @@
         <v>1.9512188925245291E-3</v>
       </c>
       <c r="J33">
-        <f t="shared" ref="J33:M33" si="38">WEIBULL(0.75,D33,E33,TRUE)</f>
+        <f t="shared" ref="J33:M33" si="40">WEIBULL(0.75,D33,E33,TRUE)</f>
         <v>1.1390560127077369E-5</v>
       </c>
       <c r="K33">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>2.3730440593264908E-6</v>
       </c>
       <c r="L33">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>4.8440629434220179E-6</v>
       </c>
       <c r="M33">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>1.768900592032779E-3</v>
       </c>
       <c r="N33">
@@ -2676,34 +2562,72 @@
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F34">
-        <v>32</v>
+        <v>0.84</v>
       </c>
       <c r="G34">
-        <v>32</v>
+        <v>0.32</v>
       </c>
       <c r="H34">
-        <v>31</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I34">
-        <f>SUM(C34:H34)</f>
-        <v>100.2</v>
+        <f>_xlfn.BINOM.INV(50,0.25,C34)</f>
+        <v>9</v>
+      </c>
+      <c r="J34">
+        <f>_xlfn.BINOM.INV(50,0.25,D34)</f>
+        <v>16</v>
+      </c>
+      <c r="K34">
+        <f>_xlfn.BINOM.INV(500,0.35,E34)</f>
+        <v>175</v>
+      </c>
+      <c r="L34">
+        <f>_xlfn.BINOM.INV(100,0.25,F34)</f>
+        <v>29</v>
+      </c>
+      <c r="M34">
+        <f>_xlfn.BINOM.INV(50,0.9,G34)</f>
+        <v>44</v>
+      </c>
+      <c r="N34">
+        <f>_xlfn.BINOM.INV(510,0.25,H34)</f>
+        <v>122</v>
+      </c>
+      <c r="O34">
+        <v>9</v>
+      </c>
+      <c r="P34">
+        <v>16</v>
+      </c>
+      <c r="Q34">
+        <v>175</v>
+      </c>
+      <c r="R34">
+        <v>29</v>
+      </c>
+      <c r="S34">
+        <v>44</v>
+      </c>
+      <c r="T34">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C35">
         <v>1.2</v>
@@ -2724,463 +2648,96 @@
         <v>31</v>
       </c>
       <c r="I35">
-        <f>SUM(C34:H35)</f>
-        <v>200.4</v>
+        <f>SUM(C35:H35)</f>
+        <v>100.2</v>
+      </c>
+      <c r="O35">
+        <v>100.2</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>1.2</v>
+      </c>
+      <c r="D36">
         <v>2</v>
       </c>
-      <c r="C36">
-        <v>0.1</v>
-      </c>
-      <c r="D36">
-        <v>0.9</v>
-      </c>
       <c r="E36">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F36">
-        <v>0.84</v>
+        <v>32</v>
       </c>
       <c r="G36">
-        <v>0.32</v>
+        <v>32</v>
       </c>
       <c r="H36">
-        <v>0.28999999999999998</v>
+        <v>31</v>
       </c>
       <c r="I36">
-        <f>_xlfn.BINOM.INV(50,0.25,C36)</f>
-        <v>9</v>
-      </c>
-      <c r="J36">
-        <f>_xlfn.BINOM.INV(50,0.25,D36)</f>
-        <v>16</v>
-      </c>
-      <c r="K36">
-        <f>_xlfn.BINOM.INV(500,0.35,E36)</f>
-        <v>175</v>
-      </c>
-      <c r="L36">
-        <f>_xlfn.BINOM.INV(100,0.25,F36)</f>
-        <v>29</v>
-      </c>
-      <c r="M36">
-        <f>_xlfn.BINOM.INV(50,0.9,G36)</f>
-        <v>44</v>
-      </c>
-      <c r="N36">
-        <f>_xlfn.BINOM.INV(510,0.25,H36)</f>
-        <v>122</v>
+        <f>SUM(C35:H36)</f>
+        <v>200.4</v>
       </c>
       <c r="O36">
-        <v>9</v>
-      </c>
-      <c r="P36">
-        <v>16</v>
-      </c>
-      <c r="Q36">
-        <v>175</v>
-      </c>
-      <c r="R36">
-        <v>29</v>
-      </c>
-      <c r="S36">
-        <v>44</v>
-      </c>
-      <c r="T36">
-        <v>122</v>
+        <v>200.4</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>43</v>
-      </c>
-      <c r="D37" t="s">
         <v>8</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37">
-        <v>21321</v>
-      </c>
-      <c r="I37" t="str">
-        <f>_xlfn.CONCAT(C37:H37)</f>
-        <v>43ABCaBC££$$test21321</v>
-      </c>
-      <c r="J37" t="str">
-        <f t="shared" ref="J37:N37" si="39">_xlfn.CONCAT(D37:I37)</f>
-        <v>ABCaBC££$$test2132143ABCaBC££$$test21321</v>
-      </c>
-      <c r="K37" t="str">
-        <f t="shared" si="39"/>
-        <v>aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</v>
-      </c>
-      <c r="L37" t="str">
-        <f t="shared" si="39"/>
-        <v>££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</v>
-      </c>
-      <c r="M37" t="str">
-        <f t="shared" si="39"/>
-        <v>test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</v>
-      </c>
-      <c r="N37" t="str">
-        <f t="shared" si="39"/>
-        <v>2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321aBC££$$test2132143ABCaBC££$$test21321ABCaBC££$$test2132143ABCaBC££$$test21321</v>
-      </c>
-      <c r="O37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P37" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>14</v>
-      </c>
-      <c r="R37" t="s">
-        <v>15</v>
-      </c>
-      <c r="S37" t="s">
-        <v>16</v>
-      </c>
-      <c r="T37" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38">
-        <v>43</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
         <v>9</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38">
-        <v>21321</v>
-      </c>
-      <c r="I38" t="str">
-        <f>CONCATENATE(C38,D38)</f>
-        <v>43ABC</v>
-      </c>
-      <c r="J38" t="str">
-        <f t="shared" ref="J38:N38" si="40">CONCATENATE(D38,E38)</f>
-        <v>ABCaBC</v>
-      </c>
-      <c r="K38" t="str">
-        <f t="shared" si="40"/>
-        <v>aBC££$$</v>
-      </c>
-      <c r="L38" t="str">
-        <f t="shared" si="40"/>
-        <v>££$$test</v>
-      </c>
-      <c r="M38" t="str">
-        <f t="shared" si="40"/>
-        <v>test21321</v>
-      </c>
-      <c r="N38" t="str">
-        <f t="shared" si="40"/>
-        <v>2132143ABC</v>
-      </c>
-      <c r="O38" t="s">
-        <v>19</v>
-      </c>
-      <c r="P38" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>21</v>
-      </c>
-      <c r="R38" t="s">
-        <v>22</v>
-      </c>
-      <c r="S38" t="s">
-        <v>23</v>
-      </c>
-      <c r="T38" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" t="s">
-        <v>57</v>
-      </c>
-      <c r="G39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I39" t="str">
-        <f>LEFT(C39,5)</f>
-        <v xml:space="preserve">Test </v>
-      </c>
-      <c r="J39" t="str">
-        <f>LEFT(D39,10)</f>
-        <v>Test and T</v>
-      </c>
-      <c r="K39" t="str">
-        <f>LEFT(E39,1)</f>
-        <v>T</v>
-      </c>
-      <c r="L39" t="str">
-        <f>LEFT(F39,15)</f>
-        <v>Test and Test</v>
-      </c>
-      <c r="M39" t="str">
-        <f>LEFT(G39,8)</f>
-        <v>Test and</v>
-      </c>
-      <c r="N39" t="str">
-        <f>LEFT(H39,2)</f>
-        <v>Te</v>
-      </c>
-      <c r="O39" t="s">
-        <v>58</v>
-      </c>
-      <c r="P39" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>60</v>
-      </c>
-      <c r="R39" t="s">
-        <v>57</v>
-      </c>
-      <c r="S39" t="s">
-        <v>61</v>
-      </c>
-      <c r="T39" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G40" t="s">
-        <v>57</v>
-      </c>
-      <c r="H40" t="s">
-        <v>57</v>
-      </c>
-      <c r="I40" t="str">
-        <f>RIGHT(C40,5)</f>
-        <v xml:space="preserve"> Test</v>
-      </c>
-      <c r="J40" t="str">
-        <f>RIGHT(D40,10)</f>
-        <v>t and Test</v>
-      </c>
-      <c r="K40" t="str">
-        <f>RIGHT(E40,1)</f>
-        <v>t</v>
-      </c>
-      <c r="L40" t="str">
-        <f>RIGHT(F40,15)</f>
-        <v>Test and Test</v>
-      </c>
-      <c r="M40" t="str">
-        <f>RIGHT(G40,8)</f>
-        <v>and Test</v>
-      </c>
-      <c r="N40" t="str">
-        <f>RIGHT(H40,2)</f>
-        <v>st</v>
-      </c>
-      <c r="O40" t="s">
-        <v>63</v>
-      </c>
-      <c r="P40" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>65</v>
-      </c>
-      <c r="R40" t="s">
-        <v>57</v>
-      </c>
-      <c r="S40" t="s">
-        <v>66</v>
-      </c>
-      <c r="T40" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" t="s">
-        <v>57</v>
-      </c>
-      <c r="E41" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" t="s">
-        <v>57</v>
-      </c>
-      <c r="G41" t="s">
-        <v>57</v>
-      </c>
-      <c r="H41" t="s">
-        <v>57</v>
-      </c>
-      <c r="I41" t="str">
-        <f>MID(C41,1,1)</f>
-        <v>T</v>
-      </c>
-      <c r="J41" t="str">
-        <f>MID(D41,4,1)</f>
-        <v>t</v>
-      </c>
-      <c r="K41" t="str">
-        <f>MID(E41,3,4)</f>
-        <v>st a</v>
-      </c>
-      <c r="L41" t="str">
-        <f>MID(F41,7,9)</f>
-        <v>nd Test</v>
-      </c>
-      <c r="M41" t="str">
-        <f>MID(G41,1,4)</f>
-        <v>Test</v>
-      </c>
-      <c r="N41" t="str">
-        <f>MID(H41,6,5)</f>
-        <v>and T</v>
-      </c>
-      <c r="O41" t="s">
-        <v>60</v>
-      </c>
-      <c r="P41" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>68</v>
-      </c>
-      <c r="R41" t="s">
-        <v>69</v>
-      </c>
-      <c r="S41" t="s">
-        <v>56</v>
-      </c>
-      <c r="T41" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update maths and stats functions
</commit_message>
<xml_diff>
--- a/reeevr/test/excelunit/reeevr-tests.xlsx
+++ b/reeevr/test/excelunit/reeevr-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mo14776\PycharmProjects\Excel-R-compiler\reeevr\test\excelunit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E25106-326D-439B-9D6E-93126752D229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AF9B98-09EA-4D8B-97BC-74214C1B5EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51741016-DE60-49DF-9826-25EB96E04CFB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Functions</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>FLOOR</t>
+  </si>
+  <si>
+    <t>CEILING</t>
   </si>
   <si>
     <t>LOG</t>
@@ -112,6 +118,36 @@
   </si>
   <si>
     <t>Val</t>
+  </si>
+  <si>
+    <t>FLOOR.MATH</t>
+  </si>
+  <si>
+    <t>CEILING.MATH</t>
+  </si>
+  <si>
+    <t>CHOOSE</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>DEGREES</t>
+  </si>
+  <si>
+    <t>RADIANS</t>
+  </si>
+  <si>
+    <t>QUARTILE</t>
+  </si>
+  <si>
+    <t>QUARTILE.INC</t>
+  </si>
+  <si>
+    <t>QUARTILE.EXC</t>
   </si>
 </sst>
 </file>
@@ -492,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1FF9ED-8125-4F1D-B85A-69D7CAC66BA2}">
-  <dimension ref="B2:T34"/>
+  <dimension ref="B2:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +559,7 @@
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -588,7 +624,7 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -978,7 +1014,7 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1043,7 +1079,7 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1108,7 +1144,7 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1173,7 +1209,7 @@
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1238,7 +1274,7 @@
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1303,7 +1339,7 @@
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1368,7 +1404,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1433,7 +1469,7 @@
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1498,7 +1534,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1563,7 +1599,7 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1628,7 +1664,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1693,7 +1729,7 @@
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1758,7 +1794,7 @@
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1823,7 +1859,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1888,7 +1924,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1953,7 +1989,7 @@
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2018,7 +2054,7 @@
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2083,7 +2119,7 @@
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2148,7 +2184,7 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2213,7 +2249,7 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2278,13 +2314,13 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -2340,13 +2376,13 @@
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -2408,10 +2444,10 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G32">
         <v>5</v>
@@ -2470,10 +2506,10 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G33">
         <v>5</v>
@@ -2538,10 +2574,10 @@
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I34">
         <f>COUNTIF(C34:H34,"&gt;3")</f>
@@ -2584,6 +2620,1512 @@
       </c>
       <c r="T34">
         <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>0.1</v>
+      </c>
+      <c r="D35">
+        <v>0.5</v>
+      </c>
+      <c r="E35">
+        <v>0.9</v>
+      </c>
+      <c r="F35">
+        <v>-0.5</v>
+      </c>
+      <c r="G35">
+        <v>-0.1</v>
+      </c>
+      <c r="H35">
+        <v>-0.9</v>
+      </c>
+      <c r="I35">
+        <f>FLOOR(C35,2)</f>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" ref="J35:N35" si="33">FLOOR(D35,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="33"/>
+        <v>-2</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="33"/>
+        <v>-2</v>
+      </c>
+      <c r="N35">
+        <f>FLOOR(H35,2)</f>
+        <v>-2</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>-2</v>
+      </c>
+      <c r="S35">
+        <v>-2</v>
+      </c>
+      <c r="T35">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>0.1</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+      <c r="E36">
+        <v>0.9</v>
+      </c>
+      <c r="F36">
+        <v>-0.5</v>
+      </c>
+      <c r="G36">
+        <v>-0.1</v>
+      </c>
+      <c r="H36">
+        <v>-0.9</v>
+      </c>
+      <c r="I36">
+        <f>FLOOR(C36,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36:N36" si="34">FLOOR(D36,1)</f>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="34"/>
+        <v>-1</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>-1</v>
+      </c>
+      <c r="S36">
+        <v>-1</v>
+      </c>
+      <c r="T36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>0.1</v>
+      </c>
+      <c r="D37">
+        <v>0.5</v>
+      </c>
+      <c r="E37">
+        <v>0.9</v>
+      </c>
+      <c r="F37">
+        <v>-0.5</v>
+      </c>
+      <c r="G37">
+        <v>-0.1</v>
+      </c>
+      <c r="H37">
+        <v>-0.9</v>
+      </c>
+      <c r="I37">
+        <f>FLOOR(C37,3)</f>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:M37" si="35">FLOOR(D37,3)</f>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="35"/>
+        <v>-3</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="35"/>
+        <v>-3</v>
+      </c>
+      <c r="N37">
+        <f>FLOOR(H37,3)</f>
+        <v>-3</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>-3</v>
+      </c>
+      <c r="S37">
+        <v>-3</v>
+      </c>
+      <c r="T37">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>3.1</v>
+      </c>
+      <c r="D38">
+        <v>5.5</v>
+      </c>
+      <c r="E38">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F38">
+        <v>-2.5</v>
+      </c>
+      <c r="G38">
+        <v>-8.1</v>
+      </c>
+      <c r="H38">
+        <v>-6.9</v>
+      </c>
+      <c r="I38">
+        <f>FLOOR(C38,2)</f>
+        <v>2</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ref="J38:N38" si="36">FLOOR(D38,2)</f>
+        <v>4</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="36"/>
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="36"/>
+        <v>-4</v>
+      </c>
+      <c r="M38">
+        <f>FLOOR(G38,2)</f>
+        <v>-10</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="36"/>
+        <v>-8</v>
+      </c>
+      <c r="O38">
+        <v>2</v>
+      </c>
+      <c r="P38">
+        <v>4</v>
+      </c>
+      <c r="Q38">
+        <v>4</v>
+      </c>
+      <c r="R38">
+        <v>-4</v>
+      </c>
+      <c r="S38">
+        <v>-10</v>
+      </c>
+      <c r="T38">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>0.1</v>
+      </c>
+      <c r="D39">
+        <v>0.5</v>
+      </c>
+      <c r="E39">
+        <v>0.9</v>
+      </c>
+      <c r="F39">
+        <v>-0.5</v>
+      </c>
+      <c r="G39">
+        <v>-0.1</v>
+      </c>
+      <c r="H39">
+        <v>-0.9</v>
+      </c>
+      <c r="I39">
+        <f>CEILING(C39,2)</f>
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <f t="shared" ref="J39:N39" si="37">CEILING(D39,2)</f>
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="37"/>
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>2</v>
+      </c>
+      <c r="P39">
+        <v>2</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>0.1</v>
+      </c>
+      <c r="D40">
+        <v>0.5</v>
+      </c>
+      <c r="E40">
+        <v>0.9</v>
+      </c>
+      <c r="F40">
+        <v>-0.5</v>
+      </c>
+      <c r="G40">
+        <v>-0.1</v>
+      </c>
+      <c r="H40">
+        <v>-0.9</v>
+      </c>
+      <c r="I40">
+        <f>CEILING(C40,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <f t="shared" ref="J40:N40" si="38">CEILING(D40,1)</f>
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>0.1</v>
+      </c>
+      <c r="D41">
+        <v>0.5</v>
+      </c>
+      <c r="E41">
+        <v>0.9</v>
+      </c>
+      <c r="F41">
+        <v>-0.5</v>
+      </c>
+      <c r="G41">
+        <v>-0.1</v>
+      </c>
+      <c r="H41">
+        <v>-0.9</v>
+      </c>
+      <c r="I41">
+        <f>CEILING(C41,3)</f>
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <f t="shared" ref="J41:N41" si="39">CEILING(D41,3)</f>
+        <v>3</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="39"/>
+        <v>3</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>3</v>
+      </c>
+      <c r="P41">
+        <v>3</v>
+      </c>
+      <c r="Q41">
+        <v>3</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>3.1</v>
+      </c>
+      <c r="D42">
+        <v>5.5</v>
+      </c>
+      <c r="E42">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F42">
+        <v>-2.5</v>
+      </c>
+      <c r="G42">
+        <v>-8.1</v>
+      </c>
+      <c r="H42">
+        <v>-6.9</v>
+      </c>
+      <c r="I42">
+        <f>CEILING(C42,2)</f>
+        <v>4</v>
+      </c>
+      <c r="J42">
+        <f t="shared" ref="J42:N42" si="40">CEILING(D42,2)</f>
+        <v>6</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="40"/>
+        <v>6</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="40"/>
+        <v>-2</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="40"/>
+        <v>-8</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="40"/>
+        <v>-6</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="P42">
+        <v>6</v>
+      </c>
+      <c r="Q42">
+        <v>6</v>
+      </c>
+      <c r="R42">
+        <v>-2</v>
+      </c>
+      <c r="S42">
+        <v>-8</v>
+      </c>
+      <c r="T42">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43">
+        <v>0.1</v>
+      </c>
+      <c r="D43">
+        <v>0.5</v>
+      </c>
+      <c r="E43">
+        <v>0.9</v>
+      </c>
+      <c r="F43">
+        <v>-0.5</v>
+      </c>
+      <c r="G43">
+        <v>-0.1</v>
+      </c>
+      <c r="H43">
+        <v>-0.9</v>
+      </c>
+      <c r="I43">
+        <f>_xlfn.FLOOR.MATH(C43,2)</f>
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <f t="shared" ref="J43:N43" si="41">_xlfn.FLOOR.MATH(D43,2)</f>
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="41"/>
+        <v>-2</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="41"/>
+        <v>-2</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="41"/>
+        <v>-2</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>-2</v>
+      </c>
+      <c r="S43">
+        <v>-2</v>
+      </c>
+      <c r="T43">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44">
+        <v>0.1</v>
+      </c>
+      <c r="D44">
+        <v>0.5</v>
+      </c>
+      <c r="E44">
+        <v>0.9</v>
+      </c>
+      <c r="F44">
+        <v>-0.5</v>
+      </c>
+      <c r="G44">
+        <v>-0.1</v>
+      </c>
+      <c r="H44">
+        <v>-0.9</v>
+      </c>
+      <c r="I44">
+        <f>_xlfn.FLOOR.MATH(C44,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ref="J44:N44" si="42">_xlfn.FLOOR.MATH(D44,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="42"/>
+        <v>-1</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="42"/>
+        <v>-1</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="42"/>
+        <v>-1</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>-1</v>
+      </c>
+      <c r="S44">
+        <v>-1</v>
+      </c>
+      <c r="T44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45">
+        <v>0.1</v>
+      </c>
+      <c r="D45">
+        <v>0.5</v>
+      </c>
+      <c r="E45">
+        <v>0.9</v>
+      </c>
+      <c r="F45">
+        <v>-0.5</v>
+      </c>
+      <c r="G45">
+        <v>-0.1</v>
+      </c>
+      <c r="H45">
+        <v>-0.9</v>
+      </c>
+      <c r="I45">
+        <f>_xlfn.FLOOR.MATH(C45,3,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <f t="shared" ref="J45:N45" si="43">_xlfn.FLOOR.MATH(D45,3,1)</f>
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46">
+        <v>3.1</v>
+      </c>
+      <c r="D46">
+        <v>5.5</v>
+      </c>
+      <c r="E46">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F46">
+        <v>-2.5</v>
+      </c>
+      <c r="G46">
+        <v>-8.1</v>
+      </c>
+      <c r="H46">
+        <v>-6.9</v>
+      </c>
+      <c r="I46">
+        <f>_xlfn.FLOOR.MATH(C46,2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46:N46" si="44">_xlfn.FLOOR.MATH(D46,2,1)</f>
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="44"/>
+        <v>4</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="44"/>
+        <v>-2</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="44"/>
+        <v>-8</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="44"/>
+        <v>-6</v>
+      </c>
+      <c r="O46">
+        <v>2</v>
+      </c>
+      <c r="P46">
+        <v>4</v>
+      </c>
+      <c r="Q46">
+        <v>4</v>
+      </c>
+      <c r="R46">
+        <v>-2</v>
+      </c>
+      <c r="S46">
+        <v>-8</v>
+      </c>
+      <c r="T46">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47">
+        <v>0.1</v>
+      </c>
+      <c r="D47">
+        <v>0.5</v>
+      </c>
+      <c r="E47">
+        <v>0.9</v>
+      </c>
+      <c r="F47">
+        <v>-0.5</v>
+      </c>
+      <c r="G47">
+        <v>-0.1</v>
+      </c>
+      <c r="H47">
+        <v>-0.9</v>
+      </c>
+      <c r="I47">
+        <f>_xlfn.CEILING.MATH(C47,2)</f>
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <f t="shared" ref="J47:N47" si="45">_xlfn.CEILING.MATH(D47,2)</f>
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+      <c r="P47">
+        <v>2</v>
+      </c>
+      <c r="Q47">
+        <v>2</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>0.1</v>
+      </c>
+      <c r="D48">
+        <v>0.5</v>
+      </c>
+      <c r="E48">
+        <v>0.9</v>
+      </c>
+      <c r="F48">
+        <v>-0.5</v>
+      </c>
+      <c r="G48">
+        <v>-0.1</v>
+      </c>
+      <c r="H48">
+        <v>-0.9</v>
+      </c>
+      <c r="I48">
+        <f>_xlfn.CEILING.MATH(C48,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <f t="shared" ref="J48:N48" si="46">_xlfn.CEILING.MATH(D48,1)</f>
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49">
+        <v>0.1</v>
+      </c>
+      <c r="D49">
+        <v>0.5</v>
+      </c>
+      <c r="E49">
+        <v>0.9</v>
+      </c>
+      <c r="F49">
+        <v>-0.5</v>
+      </c>
+      <c r="G49">
+        <v>-0.1</v>
+      </c>
+      <c r="H49">
+        <v>-0.9</v>
+      </c>
+      <c r="I49">
+        <f>_xlfn.CEILING.MATH(C49,3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49:N49" si="47">_xlfn.CEILING.MATH(D49,3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="47"/>
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>3</v>
+      </c>
+      <c r="P49">
+        <v>3</v>
+      </c>
+      <c r="Q49">
+        <v>3</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50">
+        <v>3.1</v>
+      </c>
+      <c r="D50">
+        <v>5.5</v>
+      </c>
+      <c r="E50">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F50">
+        <v>-2.5</v>
+      </c>
+      <c r="G50">
+        <v>-8.1</v>
+      </c>
+      <c r="H50">
+        <v>-6.9</v>
+      </c>
+      <c r="I50">
+        <f>_xlfn.CEILING.MATH(C50,2,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ref="J50:N50" si="48">_xlfn.CEILING.MATH(D50,2,1)</f>
+        <v>6</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="48"/>
+        <v>6</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="48"/>
+        <v>-4</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="48"/>
+        <v>-10</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="48"/>
+        <v>-8</v>
+      </c>
+      <c r="O50">
+        <v>4</v>
+      </c>
+      <c r="P50">
+        <v>6</v>
+      </c>
+      <c r="Q50">
+        <v>6</v>
+      </c>
+      <c r="R50">
+        <v>-4</v>
+      </c>
+      <c r="S50">
+        <v>-10</v>
+      </c>
+      <c r="T50">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51">
+        <v>3.1</v>
+      </c>
+      <c r="D51">
+        <v>5.5</v>
+      </c>
+      <c r="E51">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F51">
+        <v>-2.5</v>
+      </c>
+      <c r="G51">
+        <v>-8.1</v>
+      </c>
+      <c r="H51">
+        <v>-6.9</v>
+      </c>
+      <c r="I51">
+        <f>CHOOSE(1,$C51,$D51,$E51,$F51,$G51,$H51)</f>
+        <v>3.1</v>
+      </c>
+      <c r="J51">
+        <f>CHOOSE(2,$C51,$D51,$E51,$F51,$G51,$H51)</f>
+        <v>5.5</v>
+      </c>
+      <c r="K51">
+        <f>CHOOSE(3,$C51,$D51,$E51,$F51,$G51,$H51)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L51">
+        <f>CHOOSE(4,$C51,$D51,$E51,$F51,$G51,$H51)</f>
+        <v>-2.5</v>
+      </c>
+      <c r="M51">
+        <f>CHOOSE(5,$C51,$D51,$E51,$F51,$G51,$H51)</f>
+        <v>-8.1</v>
+      </c>
+      <c r="N51">
+        <f>CHOOSE(6,$C51,$D51,$E51,$F51,$G51,$H51)</f>
+        <v>-6.9</v>
+      </c>
+      <c r="O51">
+        <v>3.1</v>
+      </c>
+      <c r="P51">
+        <v>5.5</v>
+      </c>
+      <c r="Q51">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R51">
+        <v>-2.5</v>
+      </c>
+      <c r="S51">
+        <v>-8.1</v>
+      </c>
+      <c r="T51">
+        <v>-6.9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="D52">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="E52">
+        <f>PI()/3</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="F52">
+        <f>PI()*3</f>
+        <v>9.4247779607693793</v>
+      </c>
+      <c r="G52">
+        <f>PI()/6</f>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="H52">
+        <f>PI()/9</f>
+        <v>0.3490658503988659</v>
+      </c>
+      <c r="I52">
+        <f>DEGREES(C52)</f>
+        <v>180</v>
+      </c>
+      <c r="J52">
+        <f t="shared" ref="J52:N52" si="49">DEGREES(D52)</f>
+        <v>45</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="49"/>
+        <v>59.999999999999993</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="49"/>
+        <v>540</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="49"/>
+        <v>29.999999999999996</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="49"/>
+        <v>20</v>
+      </c>
+      <c r="O52">
+        <v>180</v>
+      </c>
+      <c r="P52">
+        <v>45</v>
+      </c>
+      <c r="Q52">
+        <v>59.999999999999993</v>
+      </c>
+      <c r="R52">
+        <v>540</v>
+      </c>
+      <c r="S52">
+        <v>29.999999999999996</v>
+      </c>
+      <c r="T52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53">
+        <v>90</v>
+      </c>
+      <c r="D53">
+        <v>180</v>
+      </c>
+      <c r="E53">
+        <v>60</v>
+      </c>
+      <c r="F53">
+        <v>45</v>
+      </c>
+      <c r="G53">
+        <v>270</v>
+      </c>
+      <c r="H53">
+        <v>360</v>
+      </c>
+      <c r="I53">
+        <f>RADIANS(C53)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="J53">
+        <f t="shared" ref="J53:N53" si="50">RADIANS(D53)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="50"/>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="50"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="50"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="50"/>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="O53">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="P53">
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="Q53">
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="R53">
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="S53">
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="T53">
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>-1</v>
+      </c>
+      <c r="F54">
+        <v>1.2</v>
+      </c>
+      <c r="G54">
+        <v>3.4</v>
+      </c>
+      <c r="H54">
+        <v>5.6</v>
+      </c>
+      <c r="I54">
+        <f>MAX(C54:H54)</f>
+        <v>5.6</v>
+      </c>
+      <c r="J54">
+        <f>MAX(D54:I54)</f>
+        <v>5.6</v>
+      </c>
+      <c r="K54">
+        <f>MAX(E54:J54)</f>
+        <v>5.6</v>
+      </c>
+      <c r="L54">
+        <f>MAX(F54:K54)</f>
+        <v>5.6</v>
+      </c>
+      <c r="M54">
+        <f>MAX(G54:L54)</f>
+        <v>5.6</v>
+      </c>
+      <c r="N54">
+        <f>MAX(H54:M54)</f>
+        <v>5.6</v>
+      </c>
+      <c r="O54">
+        <v>5.6</v>
+      </c>
+      <c r="P54">
+        <v>5.6</v>
+      </c>
+      <c r="Q54">
+        <v>5.6</v>
+      </c>
+      <c r="R54">
+        <v>5.6</v>
+      </c>
+      <c r="S54">
+        <v>5.6</v>
+      </c>
+      <c r="T54">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55">
+        <v>12</v>
+      </c>
+      <c r="D55">
+        <v>32</v>
+      </c>
+      <c r="E55">
+        <v>12</v>
+      </c>
+      <c r="F55">
+        <v>-1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <f>MIN(C54:H55)</f>
+        <v>-1</v>
+      </c>
+      <c r="J55">
+        <f>MIN(D54:I55)</f>
+        <v>-1</v>
+      </c>
+      <c r="K55">
+        <f>MIN(E54:J55)</f>
+        <v>-1</v>
+      </c>
+      <c r="L55">
+        <f>MIN(F54:K55)</f>
+        <v>-1</v>
+      </c>
+      <c r="M55">
+        <f>MIN(G54:L55)</f>
+        <v>-1</v>
+      </c>
+      <c r="N55">
+        <f>MIN(H54:M55)</f>
+        <v>-1</v>
+      </c>
+      <c r="O55">
+        <v>-1</v>
+      </c>
+      <c r="P55">
+        <v>-1</v>
+      </c>
+      <c r="Q55">
+        <v>-1</v>
+      </c>
+      <c r="R55">
+        <v>-1</v>
+      </c>
+      <c r="S55">
+        <v>-1</v>
+      </c>
+      <c r="T55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56">
+        <v>12</v>
+      </c>
+      <c r="D56">
+        <v>32</v>
+      </c>
+      <c r="E56">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>-1</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>3</v>
+      </c>
+      <c r="I56">
+        <f>QUARTILE($C56:$H56,0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J56">
+        <f>QUARTILE($C56:$H56,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="K56">
+        <f>QUARTILE($C56:$H56,2)</f>
+        <v>7.5</v>
+      </c>
+      <c r="L56">
+        <f>QUARTILE($C56:$H56,3)</f>
+        <v>12</v>
+      </c>
+      <c r="M56">
+        <f>QUARTILE($C56:$H56,4)</f>
+        <v>32</v>
+      </c>
+      <c r="N56">
+        <f>QUARTILE($C54:$H54,4)</f>
+        <v>5.6</v>
+      </c>
+      <c r="O56">
+        <v>-1</v>
+      </c>
+      <c r="P56">
+        <v>1.5</v>
+      </c>
+      <c r="Q56">
+        <v>7.5</v>
+      </c>
+      <c r="R56">
+        <v>12</v>
+      </c>
+      <c r="S56">
+        <v>32</v>
+      </c>
+      <c r="T56">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>32</v>
+      </c>
+      <c r="E57">
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>-1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+      <c r="I57">
+        <f>_xlfn.QUARTILE.INC($C57:$H57,0)</f>
+        <v>-1</v>
+      </c>
+      <c r="J57">
+        <f>_xlfn.QUARTILE.INC($C57:$H57,1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="K57">
+        <f>_xlfn.QUARTILE.INC($C57:$H57,2)</f>
+        <v>7.5</v>
+      </c>
+      <c r="L57">
+        <f>_xlfn.QUARTILE.INC($C57:$H57,3)</f>
+        <v>12</v>
+      </c>
+      <c r="M57">
+        <f>_xlfn.QUARTILE.INC($C57:$H57,4)</f>
+        <v>32</v>
+      </c>
+      <c r="N57">
+        <f>_xlfn.QUARTILE.INC($C54:$H54,4)</f>
+        <v>5.6</v>
+      </c>
+      <c r="O57">
+        <v>-1</v>
+      </c>
+      <c r="P57">
+        <v>1.5</v>
+      </c>
+      <c r="Q57">
+        <v>7.5</v>
+      </c>
+      <c r="R57">
+        <v>12</v>
+      </c>
+      <c r="S57">
+        <v>32</v>
+      </c>
+      <c r="T57">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>